<commit_message>
add ppoint and non-executive process to visualize
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/CompareData.xlsx
+++ b/src/main/resources/excel/CompareData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POLIGON\process-executor\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B93577C-15FE-45D6-9CD6-A27CDD69B586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA356C22-1A80-4B9D-8B26-C900F202FAA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="25100" tabRatio="343" activeTab="3" xr2:uid="{450F3A6C-B4B9-401E-BE9B-ADF9BB967B33}"/>
   </bookViews>
@@ -201,7 +201,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,6 +261,14 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -303,9 +311,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -344,9 +349,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -357,6 +359,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -673,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95F4F369-3CA8-4298-BB05-1AECDF55D2FF}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E1" activeCellId="1" sqref="A1:A14 E1:E14"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -947,7 +959,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -955,33 +967,19 @@
         <f>E17*B18</f>
         <v>400</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="27">
         <f>MIN(D2:D14)</f>
         <v>50</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18">
-        <f>SUM(E2:E15)</f>
-        <v>183</v>
-      </c>
-      <c r="F18">
-        <f>SUM(E4:E14)</f>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F19">
-        <f>SUM(E5:E14)</f>
-        <v>111</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1005,22 +1003,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1127,33 +1125,33 @@
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <f>SUM(B3:C3)</f>
         <v>54</v>
       </c>
-      <c r="C4" s="20"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="3">
         <f>SUM(D3)</f>
         <v>18</v>
       </c>
-      <c r="E4" s="20">
+      <c r="E4" s="19">
         <f>SUM(E3:G3)</f>
         <v>15</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20">
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19">
         <f>SUM(H3:J3)</f>
         <v>15</v>
       </c>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20">
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19">
         <f>SUM(K3:M3)</f>
         <v>21</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="3">
         <f>SUM(N3)</f>
         <v>60</v>
@@ -1163,61 +1161,61 @@
       <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <f>B4+D4+MAX(E4:M4)+N4</f>
         <v>153</v>
       </c>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
-      <c r="N5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <f>B5-B4</f>
         <v>99</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
     </row>
     <row r="9" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
@@ -1324,32 +1322,32 @@
       <c r="A11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B11" s="19">
         <f>SUM(B10:C10)</f>
         <v>54</v>
       </c>
-      <c r="C11" s="20"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="3">
         <f>SUM(D10)</f>
         <v>18</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="19">
         <f>SUM(E10:G10)</f>
         <v>15</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20">
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19">
         <f>SUM(H10:J10)</f>
         <v>15</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20">
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19">
         <f>SUM(K10:L10)</f>
         <v>17</v>
       </c>
-      <c r="L11" s="20"/>
+      <c r="L11" s="19"/>
       <c r="M11" s="3">
         <f>SUM(M10)</f>
         <v>4</v>
@@ -1363,78 +1361,78 @@
       <c r="A12" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <f>B11+D11+MAX(E11:M11)+N11</f>
         <v>149</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="18"/>
-      <c r="L12" s="18"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <f>B12-B11</f>
         <v>95</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="16">
+      <c r="B16" s="15">
         <f>ABS(B12-B5)/B5</f>
         <v>2.6143790849673203E-2</v>
       </c>
-      <c r="C16" s="20" t="s">
+      <c r="C16" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="12">
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="11">
         <f>B5*100</f>
         <v>15300</v>
       </c>
@@ -1443,51 +1441,46 @@
       <c r="N16" s="7"/>
     </row>
     <row r="17" spans="1:14" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <f>ABS(B13-B6)/B6</f>
         <v>4.0404040404040407E-2</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="13">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="12">
         <f>B6*100</f>
         <v>9900</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-      <c r="H19" s="22"/>
-      <c r="I19" s="22"/>
-      <c r="J19" s="22"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="K4:M4"/>
     <mergeCell ref="C16:J17"/>
     <mergeCell ref="A15:K15"/>
     <mergeCell ref="A19:N19"/>
@@ -1496,6 +1489,11 @@
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="H11:J11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="K4:M4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1506,8 +1504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745D901C-6A60-480B-B5CD-CEBF4DC351BF}">
   <dimension ref="A1:AN24"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView zoomScale="126" zoomScaleNormal="126" workbookViewId="0">
+      <selection activeCell="O40" sqref="O40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1546,118 +1544,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="21"/>
-      <c r="AE1" s="21"/>
-      <c r="AF1" s="21"/>
-      <c r="AG1" s="21"/>
-      <c r="AH1" s="21"/>
-      <c r="AI1" s="21"/>
-      <c r="AJ1" s="21"/>
-      <c r="AK1" s="21"/>
-      <c r="AL1" s="21"/>
-      <c r="AM1" s="21"/>
-      <c r="AN1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
+      <c r="AG1" s="20"/>
+      <c r="AH1" s="20"/>
+      <c r="AI1" s="20"/>
+      <c r="AJ1" s="20"/>
+      <c r="AK1" s="20"/>
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="20"/>
+      <c r="AN1" s="20"/>
     </row>
     <row r="2" spans="1:40" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20" t="s">
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20" t="s">
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20" t="s">
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20" t="s">
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20" t="s">
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20" t="s">
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20" t="s">
+      <c r="AD2" s="19"/>
+      <c r="AE2" s="19"/>
+      <c r="AF2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20" t="s">
+      <c r="AG2" s="19"/>
+      <c r="AH2" s="19"/>
+      <c r="AI2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20" t="s">
+      <c r="AJ2" s="19"/>
+      <c r="AK2" s="19"/>
+      <c r="AL2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="19"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="B3" s="3" t="s">
@@ -1904,61 +1902,61 @@
       <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21" t="s">
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21" t="s">
+      <c r="J5" s="20"/>
+      <c r="K5" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="21"/>
-      <c r="V5" s="21"/>
-      <c r="W5" s="21" t="s">
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="21"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="21"/>
-      <c r="AI5" s="21"/>
-      <c r="AJ5" s="21"/>
-      <c r="AK5" s="21"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="20"/>
+      <c r="AC5" s="20"/>
+      <c r="AD5" s="20"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="20"/>
+      <c r="AJ5" s="20"/>
+      <c r="AK5" s="20"/>
       <c r="AL5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AM5" s="21" t="s">
+      <c r="AM5" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AN5" s="21"/>
+      <c r="AN5" s="20"/>
     </row>
     <row r="6" spans="1:40" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -1967,82 +1965,82 @@
       <c r="B6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <f>C4+F4</f>
         <v>69.8</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21">
+      <c r="D6" s="19"/>
+      <c r="E6" s="20">
         <v>70.2</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="3">
         <f>I4</f>
         <v>19.7</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="20">
         <v>19.7</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="20">
+      <c r="J6" s="20"/>
+      <c r="K6" s="19">
         <f>MAX((L4+O4+R4),(U4+X4+AA4),(AD4+AG4+AJ4))</f>
         <v>28.900000000000002</v>
       </c>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="20"/>
-      <c r="W6" s="21">
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
+      <c r="O6" s="19"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="19"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="19"/>
+      <c r="V6" s="19"/>
+      <c r="W6" s="20">
         <v>29.87</v>
       </c>
-      <c r="X6" s="21"/>
-      <c r="Y6" s="21"/>
-      <c r="Z6" s="21"/>
-      <c r="AA6" s="21"/>
-      <c r="AB6" s="21"/>
-      <c r="AC6" s="21"/>
-      <c r="AD6" s="21"/>
-      <c r="AE6" s="21"/>
-      <c r="AF6" s="21"/>
-      <c r="AG6" s="21"/>
-      <c r="AH6" s="21"/>
-      <c r="AI6" s="21"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
+      <c r="Z6" s="20"/>
+      <c r="AA6" s="20"/>
+      <c r="AB6" s="20"/>
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20"/>
+      <c r="AI6" s="20"/>
       <c r="AL6" s="3">
         <f>AM4</f>
         <v>60.3</v>
       </c>
-      <c r="AM6" s="21">
+      <c r="AM6" s="20">
         <v>60.3</v>
       </c>
-      <c r="AN6" s="21"/>
+      <c r="AN6" s="20"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="22">
         <f>C6+H6+K6+AL6</f>
         <v>178.7</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="25" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="25">
+      <c r="F7" s="23">
         <v>171.9</v>
       </c>
-      <c r="G7" s="25"/>
+      <c r="G7" s="23"/>
       <c r="H7" s="9" t="s">
         <v>40</v>
       </c>
@@ -2080,169 +2078,169 @@
       <c r="AL7" s="9"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="26">
+      <c r="B8" s="22"/>
+      <c r="C8" s="24">
         <f>C7-C6</f>
         <v>108.89999999999999</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="27">
+      <c r="D8" s="24"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="25">
         <v>92.3</v>
       </c>
-      <c r="G8" s="27"/>
-      <c r="H8" s="11" t="s">
+      <c r="G8" s="25"/>
+      <c r="H8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>90</v>
       </c>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-      <c r="AB8" s="11"/>
-      <c r="AC8" s="11"/>
-      <c r="AD8" s="11"/>
-      <c r="AE8" s="11"/>
-      <c r="AF8" s="11"/>
-      <c r="AG8" s="11"/>
-      <c r="AH8" s="11"/>
-      <c r="AI8" s="11"/>
-      <c r="AJ8" s="11"/>
-      <c r="AK8" s="11"/>
-      <c r="AL8" s="11"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" s="10"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.35">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="21"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-      <c r="AC10" s="21"/>
-      <c r="AD10" s="21"/>
-      <c r="AE10" s="21"/>
-      <c r="AF10" s="21"/>
-      <c r="AG10" s="21"/>
-      <c r="AH10" s="21"/>
-      <c r="AI10" s="21"/>
-      <c r="AJ10" s="21"/>
-      <c r="AK10" s="21"/>
-      <c r="AL10" s="21"/>
-      <c r="AM10" s="21"/>
-      <c r="AN10" s="21"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
+      <c r="T10" s="20"/>
+      <c r="U10" s="20"/>
+      <c r="V10" s="20"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="20"/>
+      <c r="Y10" s="20"/>
+      <c r="Z10" s="20"/>
+      <c r="AA10" s="20"/>
+      <c r="AB10" s="20"/>
+      <c r="AC10" s="20"/>
+      <c r="AD10" s="20"/>
+      <c r="AE10" s="20"/>
+      <c r="AF10" s="20"/>
+      <c r="AG10" s="20"/>
+      <c r="AH10" s="20"/>
+      <c r="AI10" s="20"/>
+      <c r="AJ10" s="20"/>
+      <c r="AK10" s="20"/>
+      <c r="AL10" s="20"/>
+      <c r="AM10" s="20"/>
+      <c r="AN10" s="20"/>
     </row>
     <row r="11" spans="1:40" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20" t="s">
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20" t="s">
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="20" t="s">
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="O11" s="20"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="20" t="s">
+      <c r="O11" s="19"/>
+      <c r="P11" s="19"/>
+      <c r="Q11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="R11" s="20"/>
-      <c r="S11" s="20"/>
-      <c r="T11" s="20" t="s">
+      <c r="R11" s="19"/>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="U11" s="20"/>
-      <c r="V11" s="20"/>
-      <c r="W11" s="20" t="s">
+      <c r="U11" s="19"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="X11" s="20"/>
-      <c r="Y11" s="20"/>
-      <c r="Z11" s="20" t="s">
+      <c r="X11" s="19"/>
+      <c r="Y11" s="19"/>
+      <c r="Z11" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="AA11" s="20"/>
-      <c r="AB11" s="20"/>
-      <c r="AC11" s="20" t="s">
+      <c r="AA11" s="19"/>
+      <c r="AB11" s="19"/>
+      <c r="AC11" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="AD11" s="20"/>
-      <c r="AE11" s="20"/>
-      <c r="AF11" s="20" t="s">
+      <c r="AD11" s="19"/>
+      <c r="AE11" s="19"/>
+      <c r="AF11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="AG11" s="20"/>
-      <c r="AH11" s="20"/>
-      <c r="AI11" s="20" t="s">
+      <c r="AG11" s="19"/>
+      <c r="AH11" s="19"/>
+      <c r="AI11" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="AJ11" s="20"/>
-      <c r="AK11" s="20"/>
-      <c r="AL11" s="20" t="s">
+      <c r="AJ11" s="19"/>
+      <c r="AK11" s="19"/>
+      <c r="AL11" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AM11" s="20"/>
-      <c r="AN11" s="20"/>
+      <c r="AM11" s="19"/>
+      <c r="AN11" s="19"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
@@ -2489,61 +2487,61 @@
       <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21" t="s">
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
       <c r="H14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I14" s="21" t="s">
+      <c r="I14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21" t="s">
+      <c r="J14" s="20"/>
+      <c r="K14" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-      <c r="N14" s="21"/>
-      <c r="O14" s="21"/>
-      <c r="P14" s="21"/>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="21"/>
-      <c r="U14" s="21"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="21" t="s">
+      <c r="L14" s="20"/>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="20"/>
+      <c r="P14" s="20"/>
+      <c r="Q14" s="20"/>
+      <c r="R14" s="20"/>
+      <c r="S14" s="20"/>
+      <c r="T14" s="20"/>
+      <c r="U14" s="20"/>
+      <c r="V14" s="20"/>
+      <c r="W14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="X14" s="21"/>
-      <c r="Y14" s="21"/>
-      <c r="Z14" s="21"/>
-      <c r="AA14" s="21"/>
-      <c r="AB14" s="21"/>
-      <c r="AC14" s="21"/>
-      <c r="AD14" s="21"/>
-      <c r="AE14" s="21"/>
-      <c r="AF14" s="21"/>
-      <c r="AG14" s="21"/>
-      <c r="AH14" s="21"/>
-      <c r="AI14" s="21"/>
-      <c r="AJ14" s="21"/>
-      <c r="AK14" s="21"/>
+      <c r="X14" s="20"/>
+      <c r="Y14" s="20"/>
+      <c r="Z14" s="20"/>
+      <c r="AA14" s="20"/>
+      <c r="AB14" s="20"/>
+      <c r="AC14" s="20"/>
+      <c r="AD14" s="20"/>
+      <c r="AE14" s="20"/>
+      <c r="AF14" s="20"/>
+      <c r="AG14" s="20"/>
+      <c r="AH14" s="20"/>
+      <c r="AI14" s="20"/>
+      <c r="AJ14" s="20"/>
+      <c r="AK14" s="20"/>
       <c r="AL14" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AM14" s="21" t="s">
+      <c r="AM14" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="AN14" s="21"/>
+      <c r="AN14" s="20"/>
     </row>
     <row r="15" spans="1:40" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
@@ -2552,84 +2550,84 @@
       <c r="B15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="19">
         <f>C13+F13</f>
         <v>61.8</v>
       </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21">
+      <c r="D15" s="19"/>
+      <c r="E15" s="20">
         <v>62.6</v>
       </c>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
       <c r="H15" s="3">
         <f>I13</f>
         <v>19.8</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="20">
         <f>I13</f>
         <v>19.8</v>
       </c>
-      <c r="J15" s="21"/>
-      <c r="K15" s="20">
+      <c r="J15" s="20"/>
+      <c r="K15" s="19">
         <f>MAX((L13+O13+R13),(U13+X13+AA13),(AD13+AG13),AJ13)</f>
         <v>24.9</v>
       </c>
-      <c r="L15" s="20"/>
-      <c r="M15" s="20"/>
-      <c r="N15" s="20"/>
-      <c r="O15" s="20"/>
-      <c r="P15" s="20"/>
-      <c r="Q15" s="20"/>
-      <c r="R15" s="20"/>
-      <c r="S15" s="20"/>
-      <c r="T15" s="20"/>
-      <c r="U15" s="20"/>
-      <c r="V15" s="20"/>
-      <c r="W15" s="21">
+      <c r="L15" s="19"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="19"/>
+      <c r="Q15" s="19"/>
+      <c r="R15" s="19"/>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="19"/>
+      <c r="W15" s="20">
         <v>24.95</v>
       </c>
-      <c r="X15" s="21"/>
-      <c r="Y15" s="21"/>
-      <c r="Z15" s="21"/>
-      <c r="AA15" s="21"/>
-      <c r="AB15" s="21"/>
-      <c r="AC15" s="21"/>
-      <c r="AD15" s="21"/>
-      <c r="AE15" s="21"/>
-      <c r="AF15" s="21"/>
-      <c r="AG15" s="21"/>
-      <c r="AH15" s="21"/>
-      <c r="AI15" s="21"/>
+      <c r="X15" s="20"/>
+      <c r="Y15" s="20"/>
+      <c r="Z15" s="20"/>
+      <c r="AA15" s="20"/>
+      <c r="AB15" s="20"/>
+      <c r="AC15" s="20"/>
+      <c r="AD15" s="20"/>
+      <c r="AE15" s="20"/>
+      <c r="AF15" s="20"/>
+      <c r="AG15" s="20"/>
+      <c r="AH15" s="20"/>
+      <c r="AI15" s="20"/>
       <c r="AL15" s="3">
         <f>AM13</f>
         <v>60.15</v>
       </c>
-      <c r="AM15" s="21">
+      <c r="AM15" s="20">
         <f>AM13</f>
         <v>60.15</v>
       </c>
-      <c r="AN15" s="21"/>
+      <c r="AN15" s="20"/>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="22">
         <f>C15+H15+K15+AL15</f>
         <v>166.65</v>
       </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="25" t="s">
+      <c r="D16" s="22"/>
+      <c r="E16" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="25">
+      <c r="F16" s="23">
         <v>153.12</v>
       </c>
-      <c r="G16" s="25"/>
+      <c r="G16" s="23"/>
       <c r="H16" s="9" t="s">
         <v>40</v>
       </c>
@@ -2667,61 +2665,61 @@
       <c r="AL16" s="9"/>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="26">
+      <c r="B17" s="22"/>
+      <c r="C17" s="24">
         <f>C16-C15</f>
         <v>104.85000000000001</v>
       </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="27">
+      <c r="D17" s="24"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="25">
         <v>87.08</v>
       </c>
-      <c r="G17" s="27"/>
-      <c r="H17" s="11" t="s">
+      <c r="G17" s="25"/>
+      <c r="H17" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="10">
         <v>93</v>
       </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
-      <c r="AI17" s="11"/>
-      <c r="AJ17" s="11"/>
-      <c r="AK17" s="11"/>
-      <c r="AL17" s="11"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
+      <c r="R17" s="10"/>
+      <c r="S17" s="10"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10"/>
+      <c r="AJ17" s="10"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="10"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
+      <c r="A19" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="21"/>
+      <c r="B19" s="20"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -2736,11 +2734,11 @@
       <c r="A20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="16">
+      <c r="B20" s="15">
         <f>ABS(C16-C7)/C7</f>
         <v>6.7431449356463252E-2</v>
       </c>
-      <c r="C20" s="23"/>
+      <c r="C20" s="26"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -2748,17 +2746,17 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-      <c r="K20" s="12"/>
+      <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="15">
+      <c r="B21" s="14">
         <f>ABS(C17-C8)/C8</f>
         <v>3.7190082644627948E-2</v>
       </c>
-      <c r="C21" s="21"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -2766,13 +2764,63 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="13"/>
+      <c r="K21" s="12"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.35">
       <c r="M24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="66">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="W14:AK14"/>
+    <mergeCell ref="AM14:AN14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="E15:G15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="K15:V15"/>
+    <mergeCell ref="W15:AI15"/>
+    <mergeCell ref="AM15:AN15"/>
+    <mergeCell ref="K14:V14"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K5:V5"/>
+    <mergeCell ref="W5:AK5"/>
+    <mergeCell ref="K6:V6"/>
+    <mergeCell ref="W6:AI6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="AI11:AK11"/>
+    <mergeCell ref="AL11:AN11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="AL2:AN2"/>
+    <mergeCell ref="W2:Y2"/>
+    <mergeCell ref="W11:Y11"/>
+    <mergeCell ref="Z11:AB11"/>
+    <mergeCell ref="AC11:AE11"/>
+    <mergeCell ref="AF11:AH11"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AE2"/>
+    <mergeCell ref="AF2:AH2"/>
+    <mergeCell ref="AI2:AK2"/>
+    <mergeCell ref="AM5:AN5"/>
+    <mergeCell ref="AM6:AN6"/>
     <mergeCell ref="A1:AN1"/>
     <mergeCell ref="A10:AN10"/>
     <mergeCell ref="B11:D11"/>
@@ -2789,56 +2837,6 @@
     <mergeCell ref="N2:P2"/>
     <mergeCell ref="Q2:S2"/>
     <mergeCell ref="T2:V2"/>
-    <mergeCell ref="AI11:AK11"/>
-    <mergeCell ref="AL11:AN11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="AL2:AN2"/>
-    <mergeCell ref="W2:Y2"/>
-    <mergeCell ref="W11:Y11"/>
-    <mergeCell ref="Z11:AB11"/>
-    <mergeCell ref="AC11:AE11"/>
-    <mergeCell ref="AF11:AH11"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AE2"/>
-    <mergeCell ref="AF2:AH2"/>
-    <mergeCell ref="AI2:AK2"/>
-    <mergeCell ref="AM5:AN5"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K5:V5"/>
-    <mergeCell ref="W5:AK5"/>
-    <mergeCell ref="K6:V6"/>
-    <mergeCell ref="W6:AI6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="W14:AK14"/>
-    <mergeCell ref="AM14:AN14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="E15:G15"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="K15:V15"/>
-    <mergeCell ref="W15:AI15"/>
-    <mergeCell ref="AM15:AN15"/>
-    <mergeCell ref="K14:V14"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2849,7 +2847,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2863,7 +2861,7 @@
     <col min="7" max="7" width="13" style="3" customWidth="1"/>
     <col min="8" max="8" width="12.90625" style="3" customWidth="1"/>
     <col min="9" max="9" width="11.08984375" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
@@ -2871,16 +2869,16 @@
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21" t="s">
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -2910,7 +2908,7 @@
       <c r="I2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="29" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2950,7 +2948,7 @@
         <f>(G3*$B3)+(H3*$C3)</f>
         <v>10026</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="28">
         <f>(F3-I3)/F3</f>
         <v>3.9655172413793106E-2</v>
       </c>
@@ -2991,7 +2989,7 @@
         <f>(G4*$B4)+(H4*$C4)</f>
         <v>9170.2799999999988</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="18">
         <f>(F4-I4)/F4</f>
         <v>7.1646082202875189E-2</v>
       </c>
@@ -3000,11 +2998,11 @@
       <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <f>(F3-F4)/F3</f>
         <v>5.3831417624521073E-2</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="13">
         <f>(I3-I4)/I3</f>
         <v>8.5350089766606935E-2</v>
       </c>

</xml_diff>